<commit_message>
Added restart R session to R commands. Distinguished between confidence intervals / hypothesis testing for means, predicted values, and slopes.
Going to review exercises on numpy
</commit_message>
<xml_diff>
--- a/TomLeversRPackage/R_Commands.xlsx
+++ b/TomLeversRPackage/R_Commands.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Tom_Levers_Git_Repository\UVA\2--Linear_Models_For_Data_Science\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Tom_Levers_Git_Repository\TomLeversRPackage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{158F260B-2E94-4FAF-9526-04C92F569D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940EC38D-6F39-419C-8AC6-B0CE888AF5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3940" yWindow="1930" windowWidth="28800" windowHeight="15470" xr2:uid="{4113E9C0-2B3F-A842-BEAE-53D8B59B8F27}"/>
+    <workbookView xWindow="8700" yWindow="2530" windowWidth="28800" windowHeight="15470" xr2:uid="{4113E9C0-2B3F-A842-BEAE-53D8B59B8F27}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>R Commands</t>
   </si>
@@ -127,6 +127,12 @@
   <si>
     <t>install.packages("tidyverse", repos = "http://cran.us.r-project.org")
 install.packages("C:\\Users\\Tom\\Documents\\Tom_Levers_Git_Repository\\TomLeversRPackage", repos = NULL, type="source")</t>
+  </si>
+  <si>
+    <t>Restart R session</t>
+  </si>
+  <si>
+    <t>.rs.restartR()</t>
   </si>
 </sst>
 </file>
@@ -499,9 +505,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45C9CB9-7864-CD46-9303-21AF865CAB41}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -598,45 +606,54 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>15</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>